<commit_message>
Añadiendo archivos R para testeo estadistico
</commit_message>
<xml_diff>
--- a/data/datasets/IMF_GDP_per_PPA_April_2024.xlsx
+++ b/data/datasets/IMF_GDP_per_PPA_April_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dccs2\Desktop\Proyectos\Design-Complexity\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B399ABD0-E1F9-4993-B694-ABC3F8C9DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADAE7EA-111E-4A99-B788-87C475FBE2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{AD855409-C31E-4974-81DB-D0A108782E4C}"/>
   </bookViews>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48958542-2D72-4E74-BB17-62F84FDA6BAD}">
   <dimension ref="A1:X192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168:XFD168"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15916,5 +15916,6 @@
   </sheetData>
   <autoFilter ref="A1:X192" xr:uid="{48958542-2D72-4E74-BB17-62F84FDA6BAD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>